<commit_message>
Modified Practical_17 for building model topic
</commit_message>
<xml_diff>
--- a/Practical_17.xlsx
+++ b/Practical_17.xlsx
@@ -4,10 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Model Building" sheetId="1" r:id="rId1"/>
+    <sheet name="Q1" sheetId="2" r:id="rId2"/>
+    <sheet name="Q2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,9 +20,153 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
+  <si>
+    <t>Model Building</t>
+  </si>
+  <si>
+    <t>INPUT</t>
+  </si>
+  <si>
+    <t>No. of Rooms</t>
+  </si>
+  <si>
+    <t>No. of Floors</t>
+  </si>
+  <si>
+    <t>Booking Rate</t>
+  </si>
+  <si>
+    <t>Shampoo's per room</t>
+  </si>
+  <si>
+    <t>Shampoo's per night</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>How many Shampoo's are requried?</t>
+  </si>
+  <si>
+    <t>Shampoo's Required</t>
+  </si>
+  <si>
+    <t>Shampoo's Required per week</t>
+  </si>
+  <si>
+    <t>Hotel 1</t>
+  </si>
+  <si>
+    <t>Hotel 2</t>
+  </si>
+  <si>
+    <t>Hotel 3</t>
+  </si>
+  <si>
+    <t>Hotel 4</t>
+  </si>
+  <si>
+    <t>Floors</t>
+  </si>
+  <si>
+    <t>Rooms</t>
+  </si>
+  <si>
+    <t>Room's Occupied?</t>
+  </si>
+  <si>
+    <t>There are outputs below.  You will need to determine the best inputs, make assumptions for the values of the inputs, and calculate the answers.</t>
+  </si>
+  <si>
+    <t>There is no 'correct' answer here - the best answers have inputs which will allow for some flexibility, and come to an accurate answer if the assumptions are correct</t>
+  </si>
+  <si>
+    <t>Suggested answer only - yours could look different</t>
+  </si>
+  <si>
+    <t>Inputs</t>
+  </si>
+  <si>
+    <t>Outputs to solve for</t>
+  </si>
+  <si>
+    <t>Number of lightbulbs in my house</t>
+  </si>
+  <si>
+    <t>$ spent to buy bulbs for the whole house</t>
+  </si>
+  <si>
+    <t>Average $ spent on replacement bulbs per year</t>
+  </si>
+  <si>
+    <t>Golfing troubles</t>
+  </si>
+  <si>
+    <t>There are required outputs below.  You will need to determine the best inputs, make assumptions for the values of the inputs, and calculate the answers.</t>
+  </si>
+  <si>
+    <t>How much do americans spend on golf balls every year?</t>
+  </si>
+  <si>
+    <t>How many hours of golf do americans play?</t>
+  </si>
+  <si>
+    <t>How many balls would be used if everyone lost 1 fewer ball?</t>
+  </si>
+  <si>
+    <t>Floor</t>
+  </si>
+  <si>
+    <t>No. of rooms in each floor</t>
+  </si>
+  <si>
+    <t>No. of bulbs in each room</t>
+  </si>
+  <si>
+    <t>Cost of each bulb</t>
+  </si>
+  <si>
+    <t>Average life of bulb(in months)</t>
+  </si>
+  <si>
+    <t>cost of golf ball</t>
+  </si>
+  <si>
+    <t>Total population of america</t>
+  </si>
+  <si>
+    <t>people playing golf</t>
+  </si>
+  <si>
+    <t>no of games played per year</t>
+  </si>
+  <si>
+    <t>no of hours a game last</t>
+  </si>
+  <si>
+    <t>golf ball loss rate per match</t>
+  </si>
+  <si>
+    <t>no. of golf balls required per match</t>
+  </si>
+  <si>
+    <t>Total diffrence</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +174,85 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0000D7"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Garamond"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,15 +260,60 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -331,12 +591,742 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B1:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:16" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C6" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="2">
+        <v>10</v>
+      </c>
+      <c r="E8" s="2">
+        <v>20</v>
+      </c>
+      <c r="F8" s="2">
+        <v>30</v>
+      </c>
+      <c r="G8" s="2">
+        <v>40</v>
+      </c>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="2">
+        <v>8</v>
+      </c>
+      <c r="E9" s="2">
+        <v>9</v>
+      </c>
+      <c r="F9" s="2">
+        <v>10</v>
+      </c>
+      <c r="G9" s="2">
+        <v>11</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9">
+        <f>D15</f>
+        <v>112</v>
+      </c>
+      <c r="K9" s="5">
+        <v>4</v>
+      </c>
+      <c r="L9" s="5">
+        <v>5</v>
+      </c>
+      <c r="M9" s="5">
+        <v>6</v>
+      </c>
+      <c r="N9" s="5">
+        <v>7</v>
+      </c>
+      <c r="O9" s="5">
+        <v>8</v>
+      </c>
+      <c r="P9" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="I10" s="9"/>
+      <c r="J10" s="6">
+        <v>6</v>
+      </c>
+      <c r="K10">
+        <f t="dataTable" ref="K10:P16" dt2D="1" dtr="1" r1="D8" r2="D9"/>
+        <v>33.599999999999994</v>
+      </c>
+      <c r="L10">
+        <v>42</v>
+      </c>
+      <c r="M10">
+        <v>50.4</v>
+      </c>
+      <c r="N10">
+        <v>58.8</v>
+      </c>
+      <c r="O10">
+        <v>67.199999999999989</v>
+      </c>
+      <c r="P10">
+        <v>75.599999999999994</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="2">
+        <v>2</v>
+      </c>
+      <c r="E11" s="2">
+        <v>3</v>
+      </c>
+      <c r="F11" s="2">
+        <v>4</v>
+      </c>
+      <c r="G11" s="2">
+        <v>5</v>
+      </c>
+      <c r="I11" s="9"/>
+      <c r="J11" s="6">
+        <v>7</v>
+      </c>
+      <c r="K11">
+        <v>39.199999999999996</v>
+      </c>
+      <c r="L11">
+        <v>49</v>
+      </c>
+      <c r="M11">
+        <v>58.8</v>
+      </c>
+      <c r="N11">
+        <v>68.599999999999994</v>
+      </c>
+      <c r="O11">
+        <v>78.399999999999991</v>
+      </c>
+      <c r="P11">
+        <v>88.199999999999989</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2">
+        <v>2</v>
+      </c>
+      <c r="F12" s="2">
+        <v>3</v>
+      </c>
+      <c r="G12" s="2">
+        <v>4</v>
+      </c>
+      <c r="I12" s="9"/>
+      <c r="J12" s="6">
+        <v>8</v>
+      </c>
+      <c r="K12">
+        <v>44.8</v>
+      </c>
+      <c r="L12">
+        <v>56</v>
+      </c>
+      <c r="M12">
+        <v>67.199999999999989</v>
+      </c>
+      <c r="N12">
+        <v>78.399999999999991</v>
+      </c>
+      <c r="O12">
+        <v>89.6</v>
+      </c>
+      <c r="P12">
+        <v>100.8</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="I13" s="9"/>
+      <c r="J13" s="6">
+        <v>9</v>
+      </c>
+      <c r="K13">
+        <v>50.4</v>
+      </c>
+      <c r="L13">
+        <v>62.999999999999993</v>
+      </c>
+      <c r="M13">
+        <v>75.599999999999994</v>
+      </c>
+      <c r="N13">
+        <v>88.199999999999989</v>
+      </c>
+      <c r="O13">
+        <v>100.8</v>
+      </c>
+      <c r="P13">
+        <v>113.39999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I14" s="9"/>
+      <c r="J14" s="6">
+        <v>10</v>
+      </c>
+      <c r="K14">
+        <v>56</v>
+      </c>
+      <c r="L14">
+        <v>70</v>
+      </c>
+      <c r="M14">
+        <v>84</v>
+      </c>
+      <c r="N14">
+        <v>98</v>
+      </c>
+      <c r="O14">
+        <v>112</v>
+      </c>
+      <c r="P14">
+        <v>125.99999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15">
+        <f>D8*D9*D10*D11*D12</f>
+        <v>112</v>
+      </c>
+      <c r="E15">
+        <f t="shared" ref="E15:G15" si="0">E8*E9*E10*E11*E12</f>
+        <v>864</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>2880</v>
+      </c>
+      <c r="G15">
+        <f>G8*G9*G10*G11*G12</f>
+        <v>7920</v>
+      </c>
+      <c r="I15" s="9"/>
+      <c r="J15" s="6">
+        <v>11</v>
+      </c>
+      <c r="K15">
+        <v>61.599999999999994</v>
+      </c>
+      <c r="L15">
+        <v>77</v>
+      </c>
+      <c r="M15">
+        <v>92.399999999999991</v>
+      </c>
+      <c r="N15">
+        <v>107.8</v>
+      </c>
+      <c r="O15">
+        <v>123.19999999999999</v>
+      </c>
+      <c r="P15">
+        <v>138.6</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16">
+        <f>D15*7</f>
+        <v>784</v>
+      </c>
+      <c r="E16">
+        <f t="shared" ref="E16:G16" si="1">E15*7</f>
+        <v>6048</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>20160</v>
+      </c>
+      <c r="G16">
+        <f>G15*7</f>
+        <v>55440</v>
+      </c>
+      <c r="I16" s="9"/>
+      <c r="J16" s="6">
+        <v>12</v>
+      </c>
+      <c r="K16">
+        <v>67.199999999999989</v>
+      </c>
+      <c r="L16">
+        <v>84</v>
+      </c>
+      <c r="M16">
+        <v>100.8</v>
+      </c>
+      <c r="N16">
+        <v>117.6</v>
+      </c>
+      <c r="O16">
+        <v>134.39999999999998</v>
+      </c>
+      <c r="P16">
+        <v>151.19999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17">
+        <f>D8*D9*D10</f>
+        <v>56</v>
+      </c>
+      <c r="E17">
+        <f>E8*E9*E10</f>
+        <v>144</v>
+      </c>
+      <c r="F17">
+        <f t="shared" ref="E17:G17" si="2">F8*F9*F10</f>
+        <v>240</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="2"/>
+        <v>396</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="I9:I16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:Q18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+    </row>
+    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+    </row>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B9" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B10" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="2">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B11" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B12" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C13" s="13"/>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="13"/>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B15" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15">
+        <f>C9*C10*C11</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B16" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="17">
+        <f>C15*C12</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="17">
+        <f>(12/F10)*C16</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B2:P2"/>
+    <mergeCell ref="B3:Q3"/>
+    <mergeCell ref="B6:F6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:Q20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="56" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:17" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+    </row>
+    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+    </row>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B7" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="22">
+        <v>7852169842</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B8" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="23">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B9" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1564897</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B10" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B11" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B12" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B13" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B16" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="19">
+        <f>C7*C8*C9*C11*(C12+C13)</f>
+        <v>4.3007429602326968E+16</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="21">
+        <f>C7*C8*C9*C10</f>
+        <v>2457567405847255</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="19">
+        <f>C7*C8*C9*C11*(C12+C13-1)</f>
+        <v>3.6863511087708832E+16</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="17">
+        <f>C16-C18</f>
+        <v>6143918514618136</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="20">
+        <f>C19/C16</f>
+        <v>0.14285714285714279</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B3:P3"/>
+    <mergeCell ref="B4:Q4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>